<commit_message>
add table for tracking scores
</commit_message>
<xml_diff>
--- a/src/report/Final Report.xlsx
+++ b/src/report/Final Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewthomas/Desktop/Projects/MM23B/src/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2D8C0C-EF9F-2249-AA54-BC0186911C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34FAB45-9315-9C40-87A5-E820835C95BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AB3225F5-C880-4821-8576-5361D9BABD06}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="151">
   <si>
     <t>A11</t>
   </si>
@@ -470,6 +470,30 @@
   <si>
     <t>Notre Dame</t>
   </si>
+  <si>
+    <t>Round 1</t>
+  </si>
+  <si>
+    <t>Round 2</t>
+  </si>
+  <si>
+    <t>Round 3</t>
+  </si>
+  <si>
+    <t>Round 4</t>
+  </si>
+  <si>
+    <t>Round 5</t>
+  </si>
+  <si>
+    <t>Round 6</t>
+  </si>
+  <si>
+    <t>Winners</t>
+  </si>
+  <si>
+    <t>Bonuses</t>
+  </si>
 </sst>
 </file>
 
@@ -497,7 +521,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,8 +540,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -540,16 +576,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5012,10 +5076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9490B9C-02A0-4E5E-82D5-0B537101E13E}">
-  <dimension ref="B2:Y50"/>
+  <dimension ref="B2:Y56"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5045,11 +5109,11 @@
       </c>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="str">
+      <c r="B3" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!B:B, 0))</f>
         <v>Gonzaga</v>
       </c>
-      <c r="Y3" s="4" t="str">
+      <c r="Y3" s="9" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AF:AF, 0))</f>
         <v>Arizona</v>
       </c>
@@ -5070,11 +5134,11 @@
         <f>'Decision Data'!C1</f>
         <v>A12</v>
       </c>
-      <c r="D5" s="2" t="str">
+      <c r="D5" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!J:J, 0))</f>
         <v>Gonzaga</v>
       </c>
-      <c r="W5" s="2" t="str">
+      <c r="W5" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AN:AN, 0))</f>
         <v>Arizona</v>
       </c>
@@ -5088,7 +5152,7 @@
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!C:C, 0))</f>
         <v>Boise St</v>
       </c>
-      <c r="Y6" s="2" t="str">
+      <c r="Y6" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AG:AG, 0))</f>
         <v>TCU</v>
       </c>
@@ -5112,7 +5176,7 @@
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!N:N, 0))</f>
         <v>Gonzaga</v>
       </c>
-      <c r="U8" s="2" t="str">
+      <c r="U8" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AR:AR, 0))</f>
         <v>Houston</v>
       </c>
@@ -5126,7 +5190,7 @@
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!D:D, 0))</f>
         <v>Connecticut</v>
       </c>
-      <c r="Y9" s="2" t="str">
+      <c r="Y9" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AH:AH, 0))</f>
         <v>Houston</v>
       </c>
@@ -5150,7 +5214,7 @@
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!K:K, 0))</f>
         <v>Connecticut</v>
       </c>
-      <c r="W11" s="2" t="str">
+      <c r="W11" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AO:AO, 0))</f>
         <v>Houston</v>
       </c>
@@ -5160,7 +5224,7 @@
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="str">
+      <c r="B12" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!E:E, 0))</f>
         <v>Arkansas</v>
       </c>
@@ -5198,7 +5262,7 @@
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="str">
+      <c r="B15" s="10" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!F:F, 0))</f>
         <v>Alabama</v>
       </c>
@@ -5236,11 +5300,11 @@
       </c>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="str">
+      <c r="B18" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!G:G, 0))</f>
         <v>Texas Tech</v>
       </c>
-      <c r="Y18" s="2" t="str">
+      <c r="Y18" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AK:AK, 0))</f>
         <v>Tennessee</v>
       </c>
@@ -5260,7 +5324,7 @@
         <f>'Decision Data'!H1</f>
         <v>A17</v>
       </c>
-      <c r="F20" s="2" t="str">
+      <c r="F20" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!O:O, 0))</f>
         <v>Duke</v>
       </c>
@@ -5274,7 +5338,7 @@
       </c>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="str">
+      <c r="B21" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!H:H, 0))</f>
         <v>Michigan St</v>
       </c>
@@ -5306,7 +5370,7 @@
         <f>'Decision Data'!I1</f>
         <v>A18</v>
       </c>
-      <c r="D23" s="2" t="str">
+      <c r="D23" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!M:M, 0))</f>
         <v>Duke</v>
       </c>
@@ -5320,7 +5384,7 @@
       </c>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="str">
+      <c r="B24" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!I:I, 0))</f>
         <v>Duke</v>
       </c>
@@ -5332,7 +5396,7 @@
         <f>'Decision Data'!BK1</f>
         <v>E52</v>
       </c>
-      <c r="Y24" s="2" t="str">
+      <c r="Y24" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AM:AM, 0))</f>
         <v>Villanova</v>
       </c>
@@ -5358,11 +5422,11 @@
       </c>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B29" s="2" t="str">
+      <c r="B29" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!Q:Q, 0))</f>
         <v>Baylor</v>
       </c>
-      <c r="Y29" s="2" t="str">
+      <c r="Y29" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AU:AU, 0))</f>
         <v>Kansas</v>
       </c>
@@ -5386,7 +5450,7 @@
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!Y:Y, 0))</f>
         <v>Baylor</v>
       </c>
-      <c r="W31" s="2" t="str">
+      <c r="W31" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!BC:BC, 0))</f>
         <v>Kansas</v>
       </c>
@@ -5424,7 +5488,7 @@
         <f>'Decision Data'!S1</f>
         <v>B13</v>
       </c>
-      <c r="U34" s="2" t="str">
+      <c r="U34" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!BG:BG, 0))</f>
         <v>Kansas</v>
       </c>
@@ -5434,7 +5498,7 @@
       </c>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B35" s="2" t="str">
+      <c r="B35" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!S:S, 0))</f>
         <v>St Mary's CA</v>
       </c>
@@ -5458,7 +5522,7 @@
         <f>'Decision Data'!T1</f>
         <v>B14</v>
       </c>
-      <c r="D37" s="2" t="str">
+      <c r="D37" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!Z:Z, 0))</f>
         <v>UCLA</v>
       </c>
@@ -5472,7 +5536,7 @@
       </c>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B38" s="2" t="str">
+      <c r="B38" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!T:T, 0))</f>
         <v>UCLA</v>
       </c>
@@ -5534,7 +5598,7 @@
         <f>'Decision Data'!V1</f>
         <v>B16</v>
       </c>
-      <c r="D43" s="2" t="str">
+      <c r="D43" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AA:AA, 0))</f>
         <v>Purdue</v>
       </c>
@@ -5548,7 +5612,7 @@
       </c>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B44" s="2" t="str">
+      <c r="B44" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!V:V, 0))</f>
         <v>Purdue</v>
       </c>
@@ -5556,7 +5620,7 @@
         <f>'Decision Data'!AD1</f>
         <v>B32</v>
       </c>
-      <c r="Y44" s="2" t="str">
+      <c r="Y44" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!AZ:AZ, 0))</f>
         <v>Wisconsin</v>
       </c>
@@ -5628,9 +5692,104 @@
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!X:X, 0))</f>
         <v>Kentucky</v>
       </c>
-      <c r="Y50" s="2" t="str">
+      <c r="Y50" s="8" t="str">
         <f>INDEX('Decision Data'!$A:$A, MATCH(1, 'Decision Data'!BB:BB, 0))</f>
         <v>Auburn</v>
+      </c>
+    </row>
+    <row r="53" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>143</v>
+      </c>
+      <c r="I53" t="s">
+        <v>144</v>
+      </c>
+      <c r="J53" t="s">
+        <v>145</v>
+      </c>
+      <c r="K53" t="s">
+        <v>146</v>
+      </c>
+      <c r="L53" t="s">
+        <v>147</v>
+      </c>
+      <c r="M53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>149</v>
+      </c>
+      <c r="G54" s="4"/>
+      <c r="H54" s="7">
+        <v>17</v>
+      </c>
+      <c r="I54" s="7">
+        <v>7</v>
+      </c>
+      <c r="J54" s="7">
+        <v>3</v>
+      </c>
+      <c r="K54" s="7">
+        <v>0</v>
+      </c>
+      <c r="L54" s="7">
+        <v>0</v>
+      </c>
+      <c r="M54" s="7">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <f>SUMPRODUCT(H54:M54,H56:M56)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>150</v>
+      </c>
+      <c r="G55" s="5"/>
+      <c r="H55" s="7">
+        <v>1</v>
+      </c>
+      <c r="I55" s="7">
+        <v>4</v>
+      </c>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55">
+        <f>SUM(H55:M55)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>84</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
+      <c r="J56">
+        <v>5</v>
+      </c>
+      <c r="K56">
+        <v>8</v>
+      </c>
+      <c r="L56">
+        <v>13</v>
+      </c>
+      <c r="M56">
+        <v>21</v>
+      </c>
+      <c r="N56" s="6">
+        <f>SUM(N54:N55)</f>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>